<commit_message>
Horizontal alignment: Center (middle aligned) Vertical alignment: Top
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +27,10 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="15">
@@ -146,41 +150,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,100 +559,100 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="13" customWidth="1" min="11" max="11"/>
-    <col width="13" customWidth="1" min="12" max="12"/>
-    <col width="13" customWidth="1" min="13" max="13"/>
-    <col width="13" customWidth="1" min="14" max="14"/>
-    <col width="13" customWidth="1" min="15" max="15"/>
-    <col width="13" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
-    <col width="12" customWidth="1" min="18" max="18"/>
-    <col width="12" customWidth="1" min="19" max="19"/>
-    <col width="12" customWidth="1" min="20" max="20"/>
-    <col width="12" customWidth="1" min="21" max="21"/>
-    <col width="12" customWidth="1" min="22" max="22"/>
-    <col width="12" customWidth="1" min="23" max="23"/>
-    <col width="12" customWidth="1" min="24" max="24"/>
-    <col width="12" customWidth="1" min="25" max="25"/>
-    <col width="13" customWidth="1" min="26" max="26"/>
-    <col width="13" customWidth="1" min="27" max="27"/>
-    <col width="13" customWidth="1" min="28" max="28"/>
-    <col width="13" customWidth="1" min="29" max="29"/>
-    <col width="13" customWidth="1" min="30" max="30"/>
-    <col width="13" customWidth="1" min="31" max="31"/>
-    <col width="12" customWidth="1" min="32" max="32"/>
-    <col width="12" customWidth="1" min="33" max="33"/>
-    <col width="12" customWidth="1" min="34" max="34"/>
-    <col width="12" customWidth="1" min="35" max="35"/>
-    <col width="12" customWidth="1" min="36" max="36"/>
-    <col width="12" customWidth="1" min="37" max="37"/>
-    <col width="12" customWidth="1" min="38" max="38"/>
-    <col width="12" customWidth="1" min="39" max="39"/>
-    <col width="12" customWidth="1" min="40" max="40"/>
-    <col width="13" customWidth="1" min="41" max="41"/>
-    <col width="13" customWidth="1" min="42" max="42"/>
-    <col width="13" customWidth="1" min="43" max="43"/>
-    <col width="13" customWidth="1" min="44" max="44"/>
-    <col width="13" customWidth="1" min="45" max="45"/>
-    <col width="13" customWidth="1" min="46" max="46"/>
-    <col width="12" customWidth="1" min="47" max="47"/>
-    <col width="12" customWidth="1" min="48" max="48"/>
-    <col width="12" customWidth="1" min="49" max="49"/>
-    <col width="12" customWidth="1" min="50" max="50"/>
-    <col width="12" customWidth="1" min="51" max="51"/>
-    <col width="12" customWidth="1" min="52" max="52"/>
-    <col width="12" customWidth="1" min="53" max="53"/>
-    <col width="12" customWidth="1" min="54" max="54"/>
-    <col width="12" customWidth="1" min="55" max="55"/>
-    <col width="13" customWidth="1" min="56" max="56"/>
-    <col width="13" customWidth="1" min="57" max="57"/>
-    <col width="13" customWidth="1" min="58" max="58"/>
-    <col width="13" customWidth="1" min="59" max="59"/>
-    <col width="13" customWidth="1" min="60" max="60"/>
-    <col width="13" customWidth="1" min="61" max="61"/>
-    <col width="12" customWidth="1" min="62" max="62"/>
-    <col width="12" customWidth="1" min="63" max="63"/>
-    <col width="12" customWidth="1" min="64" max="64"/>
-    <col width="12" customWidth="1" min="65" max="65"/>
-    <col width="12" customWidth="1" min="66" max="66"/>
-    <col width="12" customWidth="1" min="67" max="67"/>
-    <col width="12" customWidth="1" min="68" max="68"/>
-    <col width="12" customWidth="1" min="69" max="69"/>
-    <col width="12" customWidth="1" min="70" max="70"/>
-    <col width="13" customWidth="1" min="71" max="71"/>
-    <col width="13" customWidth="1" min="72" max="72"/>
-    <col width="13" customWidth="1" min="73" max="73"/>
-    <col width="13" customWidth="1" min="74" max="74"/>
-    <col width="13" customWidth="1" min="75" max="75"/>
-    <col width="13" customWidth="1" min="76" max="76"/>
-    <col width="12" customWidth="1" min="77" max="77"/>
-    <col width="12" customWidth="1" min="78" max="78"/>
-    <col width="12" customWidth="1" min="79" max="79"/>
-    <col width="12" customWidth="1" min="80" max="80"/>
-    <col width="12" customWidth="1" min="81" max="81"/>
-    <col width="12" customWidth="1" min="82" max="82"/>
-    <col width="12" customWidth="1" min="83" max="83"/>
-    <col width="12" customWidth="1" min="84" max="84"/>
-    <col width="12" customWidth="1" min="85" max="85"/>
-    <col width="13" customWidth="1" min="86" max="86"/>
-    <col width="13" customWidth="1" min="87" max="87"/>
-    <col width="13" customWidth="1" min="88" max="88"/>
-    <col width="13" customWidth="1" min="89" max="89"/>
-    <col width="13" customWidth="1" min="90" max="90"/>
-    <col width="13" customWidth="1" min="91" max="91"/>
+    <col width="7.142857142857143" customWidth="1" min="1" max="1"/>
+    <col width="7.142857142857143" customWidth="1" min="2" max="2"/>
+    <col width="7.142857142857143" customWidth="1" min="3" max="3"/>
+    <col width="7.142857142857143" customWidth="1" min="4" max="4"/>
+    <col width="7.142857142857143" customWidth="1" min="5" max="5"/>
+    <col width="7.142857142857143" customWidth="1" min="6" max="6"/>
+    <col width="7.142857142857143" customWidth="1" min="7" max="7"/>
+    <col width="7.142857142857143" customWidth="1" min="8" max="8"/>
+    <col width="7.142857142857143" customWidth="1" min="9" max="9"/>
+    <col width="7.142857142857143" customWidth="1" min="10" max="10"/>
+    <col width="7.142857142857143" customWidth="1" min="11" max="11"/>
+    <col width="7.142857142857143" customWidth="1" min="12" max="12"/>
+    <col width="7.142857142857143" customWidth="1" min="13" max="13"/>
+    <col width="7.142857142857143" customWidth="1" min="14" max="14"/>
+    <col width="7.142857142857143" customWidth="1" min="15" max="15"/>
+    <col width="7.142857142857143" customWidth="1" min="16" max="16"/>
+    <col width="7.142857142857143" customWidth="1" min="17" max="17"/>
+    <col width="7.142857142857143" customWidth="1" min="18" max="18"/>
+    <col width="7.142857142857143" customWidth="1" min="19" max="19"/>
+    <col width="7.142857142857143" customWidth="1" min="20" max="20"/>
+    <col width="7.142857142857143" customWidth="1" min="21" max="21"/>
+    <col width="7.142857142857143" customWidth="1" min="22" max="22"/>
+    <col width="7.142857142857143" customWidth="1" min="23" max="23"/>
+    <col width="7.142857142857143" customWidth="1" min="24" max="24"/>
+    <col width="7.142857142857143" customWidth="1" min="25" max="25"/>
+    <col width="7.142857142857143" customWidth="1" min="26" max="26"/>
+    <col width="7.142857142857143" customWidth="1" min="27" max="27"/>
+    <col width="7.142857142857143" customWidth="1" min="28" max="28"/>
+    <col width="7.142857142857143" customWidth="1" min="29" max="29"/>
+    <col width="7.142857142857143" customWidth="1" min="30" max="30"/>
+    <col width="7.142857142857143" customWidth="1" min="31" max="31"/>
+    <col width="7.142857142857143" customWidth="1" min="32" max="32"/>
+    <col width="7.142857142857143" customWidth="1" min="33" max="33"/>
+    <col width="7.142857142857143" customWidth="1" min="34" max="34"/>
+    <col width="7.142857142857143" customWidth="1" min="35" max="35"/>
+    <col width="7.142857142857143" customWidth="1" min="36" max="36"/>
+    <col width="7.142857142857143" customWidth="1" min="37" max="37"/>
+    <col width="7.142857142857143" customWidth="1" min="38" max="38"/>
+    <col width="7.142857142857143" customWidth="1" min="39" max="39"/>
+    <col width="7.142857142857143" customWidth="1" min="40" max="40"/>
+    <col width="7.142857142857143" customWidth="1" min="41" max="41"/>
+    <col width="7.142857142857143" customWidth="1" min="42" max="42"/>
+    <col width="7.142857142857143" customWidth="1" min="43" max="43"/>
+    <col width="7.142857142857143" customWidth="1" min="44" max="44"/>
+    <col width="7.142857142857143" customWidth="1" min="45" max="45"/>
+    <col width="7.142857142857143" customWidth="1" min="46" max="46"/>
+    <col width="7.142857142857143" customWidth="1" min="47" max="47"/>
+    <col width="7.142857142857143" customWidth="1" min="48" max="48"/>
+    <col width="7.142857142857143" customWidth="1" min="49" max="49"/>
+    <col width="7.142857142857143" customWidth="1" min="50" max="50"/>
+    <col width="7.142857142857143" customWidth="1" min="51" max="51"/>
+    <col width="7.142857142857143" customWidth="1" min="52" max="52"/>
+    <col width="7.142857142857143" customWidth="1" min="53" max="53"/>
+    <col width="7.142857142857143" customWidth="1" min="54" max="54"/>
+    <col width="7.142857142857143" customWidth="1" min="55" max="55"/>
+    <col width="7.142857142857143" customWidth="1" min="56" max="56"/>
+    <col width="7.142857142857143" customWidth="1" min="57" max="57"/>
+    <col width="7.142857142857143" customWidth="1" min="58" max="58"/>
+    <col width="7.142857142857143" customWidth="1" min="59" max="59"/>
+    <col width="7.142857142857143" customWidth="1" min="60" max="60"/>
+    <col width="7.142857142857143" customWidth="1" min="61" max="61"/>
+    <col width="7.142857142857143" customWidth="1" min="62" max="62"/>
+    <col width="7.142857142857143" customWidth="1" min="63" max="63"/>
+    <col width="7.142857142857143" customWidth="1" min="64" max="64"/>
+    <col width="7.142857142857143" customWidth="1" min="65" max="65"/>
+    <col width="7.142857142857143" customWidth="1" min="66" max="66"/>
+    <col width="7.142857142857143" customWidth="1" min="67" max="67"/>
+    <col width="7.142857142857143" customWidth="1" min="68" max="68"/>
+    <col width="7.142857142857143" customWidth="1" min="69" max="69"/>
+    <col width="7.142857142857143" customWidth="1" min="70" max="70"/>
+    <col width="7.142857142857143" customWidth="1" min="71" max="71"/>
+    <col width="7.142857142857143" customWidth="1" min="72" max="72"/>
+    <col width="7.142857142857143" customWidth="1" min="73" max="73"/>
+    <col width="7.142857142857143" customWidth="1" min="74" max="74"/>
+    <col width="7.142857142857143" customWidth="1" min="75" max="75"/>
+    <col width="7.142857142857143" customWidth="1" min="76" max="76"/>
+    <col width="7.142857142857143" customWidth="1" min="77" max="77"/>
+    <col width="7.142857142857143" customWidth="1" min="78" max="78"/>
+    <col width="7.142857142857143" customWidth="1" min="79" max="79"/>
+    <col width="7.142857142857143" customWidth="1" min="80" max="80"/>
+    <col width="7.142857142857143" customWidth="1" min="81" max="81"/>
+    <col width="7.142857142857143" customWidth="1" min="82" max="82"/>
+    <col width="7.142857142857143" customWidth="1" min="83" max="83"/>
+    <col width="7.142857142857143" customWidth="1" min="84" max="84"/>
+    <col width="7.142857142857143" customWidth="1" min="85" max="85"/>
+    <col width="7.142857142857143" customWidth="1" min="86" max="86"/>
+    <col width="7.142857142857143" customWidth="1" min="87" max="87"/>
+    <col width="7.142857142857143" customWidth="1" min="88" max="88"/>
+    <col width="7.142857142857143" customWidth="1" min="89" max="89"/>
+    <col width="7.142857142857143" customWidth="1" min="90" max="90"/>
+    <col width="7.142857142857143" customWidth="1" min="91" max="91"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="50" customHeight="1">
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
@@ -1101,7 +1105,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="30" customHeight="1">
+    <row r="2" ht="50" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>R1</t>
@@ -1738,7 +1742,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="30" customHeight="1">
+    <row r="3" ht="50" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>R2</t>
@@ -2375,7 +2379,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="30" customHeight="1">
+    <row r="4" ht="50" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>R3</t>
@@ -3012,7 +3016,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="30" customHeight="1">
+    <row r="5" ht="50" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>R4</t>
@@ -3649,7 +3653,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="30" customHeight="1">
+    <row r="6" ht="50" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>R5</t>
@@ -4286,7 +4290,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="30" customHeight="1">
+    <row r="7" ht="50" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>R6</t>
@@ -4923,7 +4927,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="30" customHeight="1">
+    <row r="8" ht="50" customHeight="1">
       <c r="A8" s="1" t="inlineStr">
         <is>
           <t>R7</t>
@@ -5560,7 +5564,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="30" customHeight="1">
+    <row r="9" ht="50" customHeight="1">
       <c r="A9" s="1" t="inlineStr">
         <is>
           <t>R8</t>
@@ -6197,7 +6201,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="30" customHeight="1">
+    <row r="10" ht="50" customHeight="1">
       <c r="A10" s="1" t="inlineStr">
         <is>
           <t>R9</t>
@@ -6834,7 +6838,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="30" customHeight="1">
+    <row r="11" ht="50" customHeight="1">
       <c r="A11" s="1" t="inlineStr">
         <is>
           <t>R10</t>
@@ -7471,7 +7475,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="30" customHeight="1">
+    <row r="12" ht="50" customHeight="1">
       <c r="A12" s="1" t="inlineStr">
         <is>
           <t>R11</t>
@@ -8108,7 +8112,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="30" customHeight="1">
+    <row r="13" ht="50" customHeight="1">
       <c r="A13" s="1" t="inlineStr">
         <is>
           <t>R12</t>
@@ -8745,7 +8749,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="30" customHeight="1">
+    <row r="14" ht="50" customHeight="1">
       <c r="A14" s="1" t="inlineStr">
         <is>
           <t>R13</t>
@@ -9382,7 +9386,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="30" customHeight="1">
+    <row r="15" ht="50" customHeight="1">
       <c r="A15" s="1" t="inlineStr">
         <is>
           <t>R14</t>
@@ -10019,7 +10023,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="30" customHeight="1">
+    <row r="16" ht="50" customHeight="1">
       <c r="A16" s="1" t="inlineStr">
         <is>
           <t>R15</t>
@@ -10656,7 +10660,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="30" customHeight="1">
+    <row r="17" ht="50" customHeight="1">
       <c r="A17" s="1" t="inlineStr">
         <is>
           <t>R16</t>
@@ -11293,7 +11297,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="30" customHeight="1">
+    <row r="18" ht="50" customHeight="1">
       <c r="A18" s="1" t="inlineStr">
         <is>
           <t>R17</t>
@@ -11930,7 +11934,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="30" customHeight="1">
+    <row r="19" ht="50" customHeight="1">
       <c r="A19" s="1" t="inlineStr">
         <is>
           <t>R18</t>
@@ -12567,7 +12571,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="30" customHeight="1">
+    <row r="20" ht="50" customHeight="1">
       <c r="A20" s="1" t="inlineStr">
         <is>
           <t>R19</t>
@@ -13204,7 +13208,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="30" customHeight="1">
+    <row r="21" ht="50" customHeight="1">
       <c r="A21" s="1" t="inlineStr">
         <is>
           <t>R20</t>
@@ -13841,7 +13845,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="30" customHeight="1">
+    <row r="22" ht="50" customHeight="1">
       <c r="A22" s="1" t="inlineStr">
         <is>
           <t>R21</t>
@@ -14478,7 +14482,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="30" customHeight="1">
+    <row r="23" ht="50" customHeight="1">
       <c r="A23" s="1" t="inlineStr">
         <is>
           <t>R22</t>
@@ -15115,7 +15119,7 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="30" customHeight="1">
+    <row r="24" ht="50" customHeight="1">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>R23</t>
@@ -15752,7 +15756,7 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="30" customHeight="1">
+    <row r="25" ht="50" customHeight="1">
       <c r="A25" s="1" t="inlineStr">
         <is>
           <t>R24</t>
@@ -16389,7 +16393,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="30" customHeight="1">
+    <row r="26" ht="50" customHeight="1">
       <c r="A26" s="1" t="inlineStr">
         <is>
           <t>R25</t>
@@ -17026,7 +17030,7 @@
         </is>
       </c>
     </row>
-    <row r="27" ht="30" customHeight="1">
+    <row r="27" ht="50" customHeight="1">
       <c r="A27" s="1" t="inlineStr">
         <is>
           <t>R26</t>
@@ -17663,7 +17667,7 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="30" customHeight="1">
+    <row r="28" ht="50" customHeight="1">
       <c r="A28" s="1" t="inlineStr">
         <is>
           <t>R27</t>
@@ -18300,7 +18304,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="30" customHeight="1">
+    <row r="29" ht="50" customHeight="1">
       <c r="A29" s="1" t="inlineStr">
         <is>
           <t>R28</t>
@@ -18937,7 +18941,7 @@
         </is>
       </c>
     </row>
-    <row r="30" ht="30" customHeight="1">
+    <row r="30" ht="50" customHeight="1">
       <c r="A30" s="1" t="inlineStr">
         <is>
           <t>R29</t>
@@ -19574,7 +19578,7 @@
         </is>
       </c>
     </row>
-    <row r="31" ht="30" customHeight="1">
+    <row r="31" ht="50" customHeight="1">
       <c r="A31" s="1" t="inlineStr">
         <is>
           <t>R30</t>
@@ -20211,7 +20215,7 @@
         </is>
       </c>
     </row>
-    <row r="32" ht="30" customHeight="1">
+    <row r="32" ht="50" customHeight="1">
       <c r="A32" s="1" t="inlineStr">
         <is>
           <t>R31</t>
@@ -20848,7 +20852,7 @@
         </is>
       </c>
     </row>
-    <row r="33" ht="30" customHeight="1">
+    <row r="33" ht="50" customHeight="1">
       <c r="A33" s="1" t="inlineStr">
         <is>
           <t>R32</t>
@@ -21485,7 +21489,7 @@
         </is>
       </c>
     </row>
-    <row r="34" ht="30" customHeight="1">
+    <row r="34" ht="50" customHeight="1">
       <c r="A34" s="1" t="inlineStr">
         <is>
           <t>R33</t>
@@ -22122,7 +22126,7 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="30" customHeight="1">
+    <row r="35" ht="50" customHeight="1">
       <c r="A35" s="1" t="inlineStr">
         <is>
           <t>R34</t>
@@ -22759,7 +22763,7 @@
         </is>
       </c>
     </row>
-    <row r="36" ht="30" customHeight="1">
+    <row r="36" ht="50" customHeight="1">
       <c r="A36" s="1" t="inlineStr">
         <is>
           <t>R35</t>
@@ -23396,7 +23400,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="30" customHeight="1">
+    <row r="37" ht="50" customHeight="1">
       <c r="A37" s="1" t="inlineStr">
         <is>
           <t>R36</t>
@@ -24033,7 +24037,7 @@
         </is>
       </c>
     </row>
-    <row r="38" ht="30" customHeight="1">
+    <row r="38" ht="50" customHeight="1">
       <c r="A38" s="1" t="inlineStr">
         <is>
           <t>R37</t>
@@ -24670,7 +24674,7 @@
         </is>
       </c>
     </row>
-    <row r="39" ht="30" customHeight="1">
+    <row r="39" ht="50" customHeight="1">
       <c r="A39" s="1" t="inlineStr">
         <is>
           <t>R38</t>
@@ -25307,7 +25311,7 @@
         </is>
       </c>
     </row>
-    <row r="40" ht="30" customHeight="1">
+    <row r="40" ht="50" customHeight="1">
       <c r="A40" s="1" t="inlineStr">
         <is>
           <t>R39</t>
@@ -25944,7 +25948,7 @@
         </is>
       </c>
     </row>
-    <row r="41" ht="30" customHeight="1">
+    <row r="41" ht="50" customHeight="1">
       <c r="A41" s="1" t="inlineStr">
         <is>
           <t>R40</t>
@@ -26581,7 +26585,7 @@
         </is>
       </c>
     </row>
-    <row r="42" ht="30" customHeight="1">
+    <row r="42" ht="50" customHeight="1">
       <c r="A42" s="1" t="inlineStr">
         <is>
           <t>R41</t>
@@ -27218,7 +27222,7 @@
         </is>
       </c>
     </row>
-    <row r="43" ht="30" customHeight="1">
+    <row r="43" ht="50" customHeight="1">
       <c r="A43" s="1" t="inlineStr">
         <is>
           <t>R42</t>
@@ -27855,7 +27859,7 @@
         </is>
       </c>
     </row>
-    <row r="44" ht="30" customHeight="1">
+    <row r="44" ht="50" customHeight="1">
       <c r="A44" s="1" t="inlineStr">
         <is>
           <t>R43</t>
@@ -28492,7 +28496,7 @@
         </is>
       </c>
     </row>
-    <row r="45" ht="30" customHeight="1">
+    <row r="45" ht="50" customHeight="1">
       <c r="A45" s="1" t="inlineStr">
         <is>
           <t>R44</t>
@@ -29129,7 +29133,7 @@
         </is>
       </c>
     </row>
-    <row r="46" ht="30" customHeight="1">
+    <row r="46" ht="50" customHeight="1">
       <c r="A46" s="1" t="inlineStr">
         <is>
           <t>R45</t>
@@ -29766,7 +29770,7 @@
         </is>
       </c>
     </row>
-    <row r="47" ht="30" customHeight="1">
+    <row r="47" ht="50" customHeight="1">
       <c r="A47" s="1" t="inlineStr">
         <is>
           <t>R46</t>
@@ -30403,7 +30407,7 @@
         </is>
       </c>
     </row>
-    <row r="48" ht="30" customHeight="1">
+    <row r="48" ht="50" customHeight="1">
       <c r="A48" s="1" t="inlineStr">
         <is>
           <t>R47</t>
@@ -31040,7 +31044,7 @@
         </is>
       </c>
     </row>
-    <row r="49" ht="30" customHeight="1">
+    <row r="49" ht="50" customHeight="1">
       <c r="A49" s="1" t="inlineStr">
         <is>
           <t>R48</t>
@@ -31677,7 +31681,7 @@
         </is>
       </c>
     </row>
-    <row r="50" ht="30" customHeight="1">
+    <row r="50" ht="50" customHeight="1">
       <c r="A50" s="1" t="inlineStr">
         <is>
           <t>R49</t>
@@ -32314,7 +32318,7 @@
         </is>
       </c>
     </row>
-    <row r="51" ht="30" customHeight="1">
+    <row r="51" ht="50" customHeight="1">
       <c r="A51" s="1" t="inlineStr">
         <is>
           <t>R50</t>
@@ -32951,7 +32955,7 @@
         </is>
       </c>
     </row>
-    <row r="52" ht="30" customHeight="1">
+    <row r="52" ht="50" customHeight="1">
       <c r="A52" s="1" t="inlineStr">
         <is>
           <t>R51</t>
@@ -33588,7 +33592,7 @@
         </is>
       </c>
     </row>
-    <row r="53" ht="30" customHeight="1">
+    <row r="53" ht="50" customHeight="1">
       <c r="A53" s="1" t="inlineStr">
         <is>
           <t>R52</t>
@@ -34225,7 +34229,7 @@
         </is>
       </c>
     </row>
-    <row r="54" ht="30" customHeight="1">
+    <row r="54" ht="50" customHeight="1">
       <c r="A54" s="1" t="inlineStr">
         <is>
           <t>R53</t>
@@ -34862,7 +34866,7 @@
         </is>
       </c>
     </row>
-    <row r="55" ht="30" customHeight="1">
+    <row r="55" ht="50" customHeight="1">
       <c r="A55" s="1" t="inlineStr">
         <is>
           <t>R54</t>
@@ -35499,7 +35503,7 @@
         </is>
       </c>
     </row>
-    <row r="56" ht="30" customHeight="1">
+    <row r="56" ht="50" customHeight="1">
       <c r="A56" s="1" t="inlineStr">
         <is>
           <t>R55</t>
@@ -36136,7 +36140,7 @@
         </is>
       </c>
     </row>
-    <row r="57" ht="30" customHeight="1">
+    <row r="57" ht="50" customHeight="1">
       <c r="A57" s="1" t="inlineStr">
         <is>
           <t>R56</t>
@@ -36773,7 +36777,7 @@
         </is>
       </c>
     </row>
-    <row r="58" ht="30" customHeight="1">
+    <row r="58" ht="50" customHeight="1">
       <c r="A58" s="1" t="inlineStr">
         <is>
           <t>R57</t>
@@ -37410,7 +37414,7 @@
         </is>
       </c>
     </row>
-    <row r="59" ht="30" customHeight="1">
+    <row r="59" ht="50" customHeight="1">
       <c r="A59" s="1" t="inlineStr">
         <is>
           <t>R58</t>
@@ -38047,7 +38051,7 @@
         </is>
       </c>
     </row>
-    <row r="60" ht="30" customHeight="1">
+    <row r="60" ht="50" customHeight="1">
       <c r="A60" s="1" t="inlineStr">
         <is>
           <t>R59</t>
@@ -38684,7 +38688,7 @@
         </is>
       </c>
     </row>
-    <row r="61" ht="30" customHeight="1">
+    <row r="61" ht="50" customHeight="1">
       <c r="A61" s="1" t="inlineStr">
         <is>
           <t>R60</t>
@@ -39321,7 +39325,7 @@
         </is>
       </c>
     </row>
-    <row r="62" ht="30" customHeight="1">
+    <row r="62" ht="50" customHeight="1">
       <c r="A62" s="1" t="inlineStr">
         <is>
           <t>R61</t>
@@ -39958,7 +39962,7 @@
         </is>
       </c>
     </row>
-    <row r="63" ht="30" customHeight="1">
+    <row r="63" ht="50" customHeight="1">
       <c r="A63" s="1" t="inlineStr">
         <is>
           <t>R62</t>
@@ -40595,7 +40599,7 @@
         </is>
       </c>
     </row>
-    <row r="64" ht="30" customHeight="1">
+    <row r="64" ht="50" customHeight="1">
       <c r="A64" s="1" t="inlineStr">
         <is>
           <t>R63</t>
@@ -41232,7 +41236,7 @@
         </is>
       </c>
     </row>
-    <row r="65" ht="30" customHeight="1">
+    <row r="65" ht="50" customHeight="1">
       <c r="A65" s="1" t="inlineStr">
         <is>
           <t>R64</t>
@@ -41869,7 +41873,7 @@
         </is>
       </c>
     </row>
-    <row r="66" ht="30" customHeight="1">
+    <row r="66" ht="50" customHeight="1">
       <c r="A66" s="1" t="inlineStr">
         <is>
           <t>R65</t>
@@ -42506,7 +42510,7 @@
         </is>
       </c>
     </row>
-    <row r="67" ht="30" customHeight="1">
+    <row r="67" ht="50" customHeight="1">
       <c r="A67" s="1" t="inlineStr">
         <is>
           <t>R66</t>
@@ -43143,7 +43147,7 @@
         </is>
       </c>
     </row>
-    <row r="68" ht="30" customHeight="1">
+    <row r="68" ht="50" customHeight="1">
       <c r="A68" s="1" t="inlineStr">
         <is>
           <t>R67</t>
@@ -43780,7 +43784,7 @@
         </is>
       </c>
     </row>
-    <row r="69" ht="30" customHeight="1">
+    <row r="69" ht="50" customHeight="1">
       <c r="A69" s="1" t="inlineStr">
         <is>
           <t>R68</t>
@@ -44417,7 +44421,7 @@
         </is>
       </c>
     </row>
-    <row r="70" ht="30" customHeight="1">
+    <row r="70" ht="50" customHeight="1">
       <c r="A70" s="1" t="inlineStr">
         <is>
           <t>R69</t>
@@ -45054,7 +45058,7 @@
         </is>
       </c>
     </row>
-    <row r="71" ht="30" customHeight="1">
+    <row r="71" ht="50" customHeight="1">
       <c r="A71" s="1" t="inlineStr">
         <is>
           <t>R70</t>
@@ -45691,7 +45695,7 @@
         </is>
       </c>
     </row>
-    <row r="72" ht="30" customHeight="1">
+    <row r="72" ht="50" customHeight="1">
       <c r="A72" s="1" t="inlineStr">
         <is>
           <t>R71</t>
@@ -46328,7 +46332,7 @@
         </is>
       </c>
     </row>
-    <row r="73" ht="30" customHeight="1">
+    <row r="73" ht="50" customHeight="1">
       <c r="A73" s="1" t="inlineStr">
         <is>
           <t>R72</t>
@@ -46965,7 +46969,7 @@
         </is>
       </c>
     </row>
-    <row r="74" ht="30" customHeight="1">
+    <row r="74" ht="50" customHeight="1">
       <c r="A74" s="1" t="inlineStr">
         <is>
           <t>R73</t>
@@ -47602,7 +47606,7 @@
         </is>
       </c>
     </row>
-    <row r="75" ht="30" customHeight="1">
+    <row r="75" ht="50" customHeight="1">
       <c r="A75" s="1" t="inlineStr">
         <is>
           <t>R74</t>
@@ -48239,7 +48243,7 @@
         </is>
       </c>
     </row>
-    <row r="76" ht="30" customHeight="1">
+    <row r="76" ht="50" customHeight="1">
       <c r="A76" s="1" t="inlineStr">
         <is>
           <t>R75</t>
@@ -48876,7 +48880,7 @@
         </is>
       </c>
     </row>
-    <row r="77" ht="30" customHeight="1">
+    <row r="77" ht="50" customHeight="1">
       <c r="A77" s="1" t="inlineStr">
         <is>
           <t>R76</t>
@@ -49513,7 +49517,7 @@
         </is>
       </c>
     </row>
-    <row r="78" ht="30" customHeight="1">
+    <row r="78" ht="50" customHeight="1">
       <c r="A78" s="1" t="inlineStr">
         <is>
           <t>R77</t>
@@ -50150,7 +50154,7 @@
         </is>
       </c>
     </row>
-    <row r="79" ht="30" customHeight="1">
+    <row r="79" ht="50" customHeight="1">
       <c r="A79" s="1" t="inlineStr">
         <is>
           <t>R78</t>
@@ -50787,7 +50791,7 @@
         </is>
       </c>
     </row>
-    <row r="80" ht="30" customHeight="1">
+    <row r="80" ht="50" customHeight="1">
       <c r="A80" s="1" t="inlineStr">
         <is>
           <t>R79</t>
@@ -51424,7 +51428,7 @@
         </is>
       </c>
     </row>
-    <row r="81" ht="30" customHeight="1">
+    <row r="81" ht="50" customHeight="1">
       <c r="A81" s="1" t="inlineStr">
         <is>
           <t>R80</t>
@@ -52061,7 +52065,7 @@
         </is>
       </c>
     </row>
-    <row r="82" ht="30" customHeight="1">
+    <row r="82" ht="50" customHeight="1">
       <c r="A82" s="1" t="inlineStr">
         <is>
           <t>R81</t>
@@ -52698,7 +52702,7 @@
         </is>
       </c>
     </row>
-    <row r="83" ht="30" customHeight="1">
+    <row r="83" ht="50" customHeight="1">
       <c r="A83" s="1" t="inlineStr">
         <is>
           <t>R82</t>
@@ -53335,7 +53339,7 @@
         </is>
       </c>
     </row>
-    <row r="84" ht="30" customHeight="1">
+    <row r="84" ht="50" customHeight="1">
       <c r="A84" s="1" t="inlineStr">
         <is>
           <t>R83</t>
@@ -53972,7 +53976,7 @@
         </is>
       </c>
     </row>
-    <row r="85" ht="30" customHeight="1">
+    <row r="85" ht="50" customHeight="1">
       <c r="A85" s="1" t="inlineStr">
         <is>
           <t>R84</t>
@@ -54609,7 +54613,7 @@
         </is>
       </c>
     </row>
-    <row r="86" ht="30" customHeight="1">
+    <row r="86" ht="50" customHeight="1">
       <c r="A86" s="1" t="inlineStr">
         <is>
           <t>R85</t>
@@ -55246,7 +55250,7 @@
         </is>
       </c>
     </row>
-    <row r="87" ht="30" customHeight="1">
+    <row r="87" ht="50" customHeight="1">
       <c r="A87" s="1" t="inlineStr">
         <is>
           <t>R86</t>
@@ -55883,7 +55887,7 @@
         </is>
       </c>
     </row>
-    <row r="88" ht="30" customHeight="1">
+    <row r="88" ht="50" customHeight="1">
       <c r="A88" s="1" t="inlineStr">
         <is>
           <t>R87</t>
@@ -56520,7 +56524,7 @@
         </is>
       </c>
     </row>
-    <row r="89" ht="30" customHeight="1">
+    <row r="89" ht="50" customHeight="1">
       <c r="A89" s="1" t="inlineStr">
         <is>
           <t>R88</t>
@@ -57157,7 +57161,7 @@
         </is>
       </c>
     </row>
-    <row r="90" ht="30" customHeight="1">
+    <row r="90" ht="50" customHeight="1">
       <c r="A90" s="1" t="inlineStr">
         <is>
           <t>R89</t>
@@ -57794,7 +57798,7 @@
         </is>
       </c>
     </row>
-    <row r="91" ht="30" customHeight="1">
+    <row r="91" ht="50" customHeight="1">
       <c r="A91" s="1" t="inlineStr">
         <is>
           <t>R90</t>
@@ -58431,7 +58435,7 @@
         </is>
       </c>
     </row>
-    <row r="92" ht="30" customHeight="1">
+    <row r="92" ht="50" customHeight="1">
       <c r="A92" s="1" t="inlineStr">
         <is>
           <t>R91</t>
@@ -59068,7 +59072,7 @@
         </is>
       </c>
     </row>
-    <row r="93" ht="30" customHeight="1">
+    <row r="93" ht="50" customHeight="1">
       <c r="A93" s="1" t="inlineStr">
         <is>
           <t>R92</t>
@@ -59705,7 +59709,7 @@
         </is>
       </c>
     </row>
-    <row r="94" ht="30" customHeight="1">
+    <row r="94" ht="50" customHeight="1">
       <c r="A94" s="1" t="inlineStr">
         <is>
           <t>R93</t>
@@ -60342,7 +60346,7 @@
         </is>
       </c>
     </row>
-    <row r="95" ht="30" customHeight="1">
+    <row r="95" ht="50" customHeight="1">
       <c r="A95" s="1" t="inlineStr">
         <is>
           <t>R94</t>
@@ -60979,7 +60983,7 @@
         </is>
       </c>
     </row>
-    <row r="96" ht="30" customHeight="1">
+    <row r="96" ht="50" customHeight="1">
       <c r="A96" s="1" t="inlineStr">
         <is>
           <t>R95</t>
@@ -61616,7 +61620,7 @@
         </is>
       </c>
     </row>
-    <row r="97" ht="30" customHeight="1">
+    <row r="97" ht="50" customHeight="1">
       <c r="A97" s="1" t="inlineStr">
         <is>
           <t>R96</t>
@@ -62253,7 +62257,7 @@
         </is>
       </c>
     </row>
-    <row r="98" ht="30" customHeight="1">
+    <row r="98" ht="50" customHeight="1">
       <c r="A98" s="1" t="inlineStr">
         <is>
           <t>R97</t>
@@ -62890,7 +62894,7 @@
         </is>
       </c>
     </row>
-    <row r="99" ht="30" customHeight="1">
+    <row r="99" ht="50" customHeight="1">
       <c r="A99" s="1" t="inlineStr">
         <is>
           <t>R98</t>
@@ -63527,7 +63531,7 @@
         </is>
       </c>
     </row>
-    <row r="100" ht="30" customHeight="1">
+    <row r="100" ht="50" customHeight="1">
       <c r="A100" s="1" t="inlineStr">
         <is>
           <t>R99</t>
@@ -64164,7 +64168,7 @@
         </is>
       </c>
     </row>
-    <row r="101" ht="30" customHeight="1">
+    <row r="101" ht="50" customHeight="1">
       <c r="A101" s="1" t="inlineStr">
         <is>
           <t>R100</t>
@@ -64801,7 +64805,7 @@
         </is>
       </c>
     </row>
-    <row r="102" ht="30" customHeight="1">
+    <row r="102" ht="50" customHeight="1">
       <c r="A102" s="1" t="inlineStr">
         <is>
           <t>R101</t>
@@ -65438,7 +65442,7 @@
         </is>
       </c>
     </row>
-    <row r="103" ht="30" customHeight="1">
+    <row r="103" ht="50" customHeight="1">
       <c r="A103" s="1" t="inlineStr">
         <is>
           <t>R102</t>
@@ -66075,7 +66079,7 @@
         </is>
       </c>
     </row>
-    <row r="104" ht="30" customHeight="1">
+    <row r="104" ht="50" customHeight="1">
       <c r="A104" s="1" t="inlineStr">
         <is>
           <t>R103</t>
@@ -66712,7 +66716,7 @@
         </is>
       </c>
     </row>
-    <row r="105" ht="30" customHeight="1">
+    <row r="105" ht="50" customHeight="1">
       <c r="A105" s="1" t="inlineStr">
         <is>
           <t>R104</t>
@@ -67349,7 +67353,7 @@
         </is>
       </c>
     </row>
-    <row r="106" ht="30" customHeight="1">
+    <row r="106" ht="50" customHeight="1">
       <c r="A106" s="1" t="inlineStr">
         <is>
           <t>R105</t>
@@ -67986,7 +67990,7 @@
         </is>
       </c>
     </row>
-    <row r="107" ht="30" customHeight="1">
+    <row r="107" ht="50" customHeight="1">
       <c r="A107" s="1" t="inlineStr">
         <is>
           <t>R106</t>
@@ -68623,7 +68627,7 @@
         </is>
       </c>
     </row>
-    <row r="108" ht="30" customHeight="1">
+    <row r="108" ht="50" customHeight="1">
       <c r="A108" s="1" t="inlineStr">
         <is>
           <t>R107</t>
@@ -69260,7 +69264,7 @@
         </is>
       </c>
     </row>
-    <row r="109" ht="30" customHeight="1">
+    <row r="109" ht="50" customHeight="1">
       <c r="A109" s="1" t="inlineStr">
         <is>
           <t>R108</t>
@@ -69897,7 +69901,7 @@
         </is>
       </c>
     </row>
-    <row r="110" ht="30" customHeight="1">
+    <row r="110" ht="50" customHeight="1">
       <c r="A110" s="1" t="inlineStr">
         <is>
           <t>R109</t>
@@ -70534,7 +70538,7 @@
         </is>
       </c>
     </row>
-    <row r="111" ht="30" customHeight="1">
+    <row r="111" ht="50" customHeight="1">
       <c r="A111" s="1" t="inlineStr">
         <is>
           <t>R110</t>
@@ -71171,7 +71175,7 @@
         </is>
       </c>
     </row>
-    <row r="112" ht="30" customHeight="1">
+    <row r="112" ht="50" customHeight="1">
       <c r="A112" s="1" t="inlineStr">
         <is>
           <t>R111</t>
@@ -71808,7 +71812,7 @@
         </is>
       </c>
     </row>
-    <row r="113" ht="30" customHeight="1">
+    <row r="113" ht="50" customHeight="1">
       <c r="A113" s="1" t="inlineStr">
         <is>
           <t>R112</t>
@@ -72445,7 +72449,7 @@
         </is>
       </c>
     </row>
-    <row r="114" ht="30" customHeight="1">
+    <row r="114" ht="50" customHeight="1">
       <c r="A114" s="1" t="inlineStr">
         <is>
           <t>R113</t>
@@ -73082,7 +73086,7 @@
         </is>
       </c>
     </row>
-    <row r="115" ht="30" customHeight="1">
+    <row r="115" ht="50" customHeight="1">
       <c r="A115" s="1" t="inlineStr">
         <is>
           <t>R114</t>
@@ -73719,7 +73723,7 @@
         </is>
       </c>
     </row>
-    <row r="116" ht="30" customHeight="1">
+    <row r="116" ht="50" customHeight="1">
       <c r="A116" s="1" t="inlineStr">
         <is>
           <t>R115</t>
@@ -74356,7 +74360,7 @@
         </is>
       </c>
     </row>
-    <row r="117" ht="30" customHeight="1">
+    <row r="117" ht="50" customHeight="1">
       <c r="A117" s="1" t="inlineStr">
         <is>
           <t>R116</t>
@@ -74993,7 +74997,7 @@
         </is>
       </c>
     </row>
-    <row r="118" ht="30" customHeight="1">
+    <row r="118" ht="50" customHeight="1">
       <c r="A118" s="1" t="inlineStr">
         <is>
           <t>R117</t>
@@ -75630,7 +75634,7 @@
         </is>
       </c>
     </row>
-    <row r="119" ht="30" customHeight="1">
+    <row r="119" ht="50" customHeight="1">
       <c r="A119" s="1" t="inlineStr">
         <is>
           <t>R118</t>
@@ -76267,7 +76271,7 @@
         </is>
       </c>
     </row>
-    <row r="120" ht="30" customHeight="1">
+    <row r="120" ht="50" customHeight="1">
       <c r="A120" s="1" t="inlineStr">
         <is>
           <t>R119</t>
@@ -76904,7 +76908,7 @@
         </is>
       </c>
     </row>
-    <row r="121" ht="30" customHeight="1">
+    <row r="121" ht="50" customHeight="1">
       <c r="A121" s="1" t="inlineStr">
         <is>
           <t>R120</t>

</xml_diff>